<commit_message>
Add author information for "Introduction to Information Network I"
</commit_message>
<xml_diff>
--- a/chiloPro/common/authors.xlsx
+++ b/chiloPro/common/authors.xlsx
@@ -5,17 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHiLO-Producer\chiloPro\common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chilo-producer\chiloPro\common\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11070" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11070" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sample" sheetId="6" r:id="rId1"/>
+    <sheet name="日置慎治" sheetId="10" r:id="rId1"/>
     <sheet name="Template" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>picture</t>
     <phoneticPr fontId="1"/>
@@ -127,22 +127,56 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>organization</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Masumi Hori</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>015_photo.jpg</t>
+    <t>001_photo.png</t>
+  </si>
+  <si>
+    <t>HIOKI, Shinji</t>
+  </si>
+  <si>
+    <t>帝塚山大学経営学部教授</t>
+  </si>
+  <si>
+    <t>博士（工学）</t>
+  </si>
+  <si>
+    <t>学位</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大阪大学基礎工学研究科数理専攻博士後期課程修了。工学博士。 広島大学理学部助手等を経て、現在、帝塚山大学経営学部教授、学部長。ゴードン・ベル賞受賞（1995）</t>
+  </si>
+  <si>
+    <t>物理学 / 素粒子・原子核・宇宙線・宇宙物理 / 情報学 / 図書館情報学・人文社会情報学</t>
+  </si>
+  <si>
+    <t>シミュレーション(292) , 格子QCD(4) , 数値シミュレ-ション(94) , ハドロン(12) , 並列計算(50) , 有限温度質量(1) , 質量移行(1) , ハイパフォ-マンス(1) , ハイパフォ-マンスコンピュ-ティング(20) , ス-パ-コンピュ-タ(11) , 有限温度(2) , クオ-ク・グル-ホン・プラズマ(1) , 質量(6) , トポロジ-(44) , 格子色力学(QCD)(1) , モンテカルロシミュレ-ション(25) , 人口(29) , グルーオン(5) , インターネット(219) , 江戸時代(19)</t>
+  </si>
+  <si>
+    <t>【専門分野】</t>
+    <rPh sb="1" eb="3">
+      <t>センモン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ブンヤ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>【研究キーワード】</t>
+    <rPh sb="1" eb="3">
+      <t>ケンキュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日置 慎治</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -793,7 +827,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -808,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>4</v>
@@ -822,7 +858,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>5</v>
@@ -835,7 +871,9 @@
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
@@ -843,35 +881,51 @@
     </row>
     <row r="4" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C6" s="14"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="99.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
     </row>
@@ -883,11 +937,6 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -895,9 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>